<commit_message>
_ change kpi file
</commit_message>
<xml_diff>
--- a/src/assets/resource/5002_KPIs Performance Report_202004_PBO_089_Final.xlsx
+++ b/src/assets/resource/5002_KPIs Performance Report_202004_PBO_089_Final.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hungm\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\salesapp-portal\src\assets\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -437,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -599,6 +599,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -650,17 +662,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -879,8 +882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H11" workbookViewId="0">
-      <selection activeCell="Z16" sqref="Z16"/>
+    <sheetView tabSelected="1" topLeftCell="O11" workbookViewId="0">
+      <selection activeCell="AC13" sqref="AC13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -906,19 +909,19 @@
   <sheetData>
     <row r="1" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="48"/>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="44"/>
       <c r="F1" s="44"/>
       <c r="G1" s="44"/>
       <c r="H1" s="45"/>
-      <c r="I1" s="66" t="s">
+      <c r="I1" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="67"/>
+      <c r="J1" s="71"/>
       <c r="K1" s="4"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -946,17 +949,17 @@
     </row>
     <row r="2" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="43"/>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
       <c r="H2" s="52"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="69"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="73"/>
       <c r="K2" s="4"/>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
@@ -984,17 +987,17 @@
     </row>
     <row r="3" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="49"/>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="16"/>
       <c r="H3" s="53"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="69"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="73"/>
       <c r="K3" s="4"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
@@ -1022,17 +1025,17 @@
     </row>
     <row r="4" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="50"/>
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="16"/>
       <c r="H4" s="53"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="69"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="73"/>
       <c r="K4" s="4"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
@@ -1067,8 +1070,8 @@
       <c r="F5" s="13"/>
       <c r="G5" s="16"/>
       <c r="H5" s="53"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="69"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="73"/>
       <c r="K5" s="4"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
@@ -1095,54 +1098,54 @@
       <c r="AH5" s="46"/>
     </row>
     <row r="6" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="69"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="73"/>
     </row>
     <row r="7" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="60" t="s">
+      <c r="A7" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="68"/>
-      <c r="J7" s="69"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="73"/>
     </row>
     <row r="8" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="63" t="s">
+      <c r="A8" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="64"/>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="65"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="71"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="69"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="75"/>
     </row>
     <row r="12" spans="1:34" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="59" t="s">
+      <c r="A12" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="59"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="63"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="7"/>
@@ -1304,24 +1307,24 @@
       <c r="I16" s="28"/>
       <c r="J16" s="29"/>
       <c r="K16" s="30"/>
-      <c r="L16" s="56" t="s">
+      <c r="L16" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="M16" s="56"/>
-      <c r="N16" s="56"/>
-      <c r="O16" s="56"/>
-      <c r="P16" s="56"/>
-      <c r="Q16" s="56"/>
-      <c r="R16" s="73" t="s">
+      <c r="M16" s="60"/>
+      <c r="N16" s="60"/>
+      <c r="O16" s="60"/>
+      <c r="P16" s="60"/>
+      <c r="Q16" s="60"/>
+      <c r="R16" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="S16" s="74"/>
-      <c r="T16" s="74"/>
-      <c r="U16" s="74"/>
-      <c r="V16" s="74"/>
-      <c r="W16" s="74"/>
-      <c r="X16" s="74"/>
-      <c r="Y16" s="74"/>
+      <c r="S16" s="56"/>
+      <c r="T16" s="56"/>
+      <c r="U16" s="56"/>
+      <c r="V16" s="56"/>
+      <c r="W16" s="56"/>
+      <c r="X16" s="56"/>
+      <c r="Y16" s="56"/>
     </row>
     <row r="17" spans="1:34" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
@@ -1335,30 +1338,30 @@
       <c r="I17" s="28"/>
       <c r="J17" s="29"/>
       <c r="K17" s="30"/>
-      <c r="L17" s="55" t="s">
+      <c r="L17" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="M17" s="55"/>
-      <c r="N17" s="55"/>
-      <c r="O17" s="55" t="s">
+      <c r="M17" s="59"/>
+      <c r="N17" s="59"/>
+      <c r="O17" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="P17" s="55"/>
-      <c r="Q17" s="55"/>
-      <c r="R17" s="73" t="s">
+      <c r="P17" s="59"/>
+      <c r="Q17" s="59"/>
+      <c r="R17" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="S17" s="74"/>
-      <c r="T17" s="74"/>
-      <c r="U17" s="74"/>
-      <c r="V17" s="72" t="s">
+      <c r="S17" s="56"/>
+      <c r="T17" s="56"/>
+      <c r="U17" s="56"/>
+      <c r="V17" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="W17" s="72"/>
-      <c r="X17" s="75" t="s">
+      <c r="W17" s="57"/>
+      <c r="X17" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="Y17" s="75"/>
+      <c r="Y17" s="58"/>
     </row>
     <row r="18" spans="1:34" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
@@ -1524,8 +1527,8 @@
       <c r="Y19" s="6">
         <v>52954810.333279997</v>
       </c>
-      <c r="Z19" s="6">
-        <v>70</v>
+      <c r="Z19" s="76">
+        <v>0.7</v>
       </c>
       <c r="AA19" s="6"/>
       <c r="AB19" s="6"/>
@@ -1612,8 +1615,8 @@
       <c r="Y20" s="6">
         <v>0</v>
       </c>
-      <c r="Z20" s="6">
-        <v>80</v>
+      <c r="Z20" s="76">
+        <v>0.8</v>
       </c>
       <c r="AA20" s="6"/>
       <c r="AB20" s="6"/>
@@ -8760,13 +8763,7 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="R16:Y16"/>
-    <mergeCell ref="R17:U17"/>
-    <mergeCell ref="V17:W17"/>
-    <mergeCell ref="X17:Y17"/>
-    <mergeCell ref="L17:N17"/>
-    <mergeCell ref="O17:Q17"/>
-    <mergeCell ref="L16:Q16"/>
+    <mergeCell ref="I1:J8"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
@@ -8775,7 +8772,13 @@
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="A8:H8"/>
-    <mergeCell ref="I1:J8"/>
+    <mergeCell ref="R16:Y16"/>
+    <mergeCell ref="R17:U17"/>
+    <mergeCell ref="V17:W17"/>
+    <mergeCell ref="X17:Y17"/>
+    <mergeCell ref="L17:N17"/>
+    <mergeCell ref="O17:Q17"/>
+    <mergeCell ref="L16:Q16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert "_ change kpi file"
This reverts commit f4a7aba23bde3ce64d887b8b2ee7453f812b1245
</commit_message>
<xml_diff>
--- a/src/assets/resource/5002_KPIs Performance Report_202004_PBO_089_Final.xlsx
+++ b/src/assets/resource/5002_KPIs Performance Report_202004_PBO_089_Final.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\salesapp-portal\src\assets\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hungm\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -437,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -599,18 +599,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -662,8 +650,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -882,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O11" workbookViewId="0">
-      <selection activeCell="AC13" sqref="AC13"/>
+    <sheetView tabSelected="1" topLeftCell="H11" workbookViewId="0">
+      <selection activeCell="Z16" sqref="Z16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -909,19 +906,19 @@
   <sheetData>
     <row r="1" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="48"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
       <c r="E1" s="44"/>
       <c r="F1" s="44"/>
       <c r="G1" s="44"/>
       <c r="H1" s="45"/>
-      <c r="I1" s="70" t="s">
+      <c r="I1" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="71"/>
+      <c r="J1" s="67"/>
       <c r="K1" s="4"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -949,17 +946,17 @@
     </row>
     <row r="2" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="43"/>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
       <c r="H2" s="52"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="73"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="69"/>
       <c r="K2" s="4"/>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
@@ -987,17 +984,17 @@
     </row>
     <row r="3" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="49"/>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="16"/>
       <c r="H3" s="53"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="73"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="69"/>
       <c r="K3" s="4"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
@@ -1025,17 +1022,17 @@
     </row>
     <row r="4" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="50"/>
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="16"/>
       <c r="H4" s="53"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="73"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="69"/>
       <c r="K4" s="4"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
@@ -1070,8 +1067,8 @@
       <c r="F5" s="13"/>
       <c r="G5" s="16"/>
       <c r="H5" s="53"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="73"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="69"/>
       <c r="K5" s="4"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
@@ -1098,54 +1095,54 @@
       <c r="AH5" s="46"/>
     </row>
     <row r="6" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="73"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="69"/>
     </row>
     <row r="7" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="65"/>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="66"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="73"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="69"/>
     </row>
     <row r="8" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="67" t="s">
+      <c r="A8" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="74"/>
-      <c r="J8" s="75"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="70"/>
+      <c r="J8" s="71"/>
     </row>
     <row r="12" spans="1:34" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="63" t="s">
+      <c r="A12" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="63"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="63"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="7"/>
@@ -1307,24 +1304,24 @@
       <c r="I16" s="28"/>
       <c r="J16" s="29"/>
       <c r="K16" s="30"/>
-      <c r="L16" s="60" t="s">
+      <c r="L16" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="M16" s="60"/>
-      <c r="N16" s="60"/>
-      <c r="O16" s="60"/>
-      <c r="P16" s="60"/>
-      <c r="Q16" s="60"/>
-      <c r="R16" s="55" t="s">
+      <c r="M16" s="56"/>
+      <c r="N16" s="56"/>
+      <c r="O16" s="56"/>
+      <c r="P16" s="56"/>
+      <c r="Q16" s="56"/>
+      <c r="R16" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="S16" s="56"/>
-      <c r="T16" s="56"/>
-      <c r="U16" s="56"/>
-      <c r="V16" s="56"/>
-      <c r="W16" s="56"/>
-      <c r="X16" s="56"/>
-      <c r="Y16" s="56"/>
+      <c r="S16" s="74"/>
+      <c r="T16" s="74"/>
+      <c r="U16" s="74"/>
+      <c r="V16" s="74"/>
+      <c r="W16" s="74"/>
+      <c r="X16" s="74"/>
+      <c r="Y16" s="74"/>
     </row>
     <row r="17" spans="1:34" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
@@ -1338,30 +1335,30 @@
       <c r="I17" s="28"/>
       <c r="J17" s="29"/>
       <c r="K17" s="30"/>
-      <c r="L17" s="59" t="s">
+      <c r="L17" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="M17" s="59"/>
-      <c r="N17" s="59"/>
-      <c r="O17" s="59" t="s">
+      <c r="M17" s="55"/>
+      <c r="N17" s="55"/>
+      <c r="O17" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="P17" s="59"/>
-      <c r="Q17" s="59"/>
-      <c r="R17" s="55" t="s">
+      <c r="P17" s="55"/>
+      <c r="Q17" s="55"/>
+      <c r="R17" s="73" t="s">
         <v>57</v>
       </c>
-      <c r="S17" s="56"/>
-      <c r="T17" s="56"/>
-      <c r="U17" s="56"/>
-      <c r="V17" s="57" t="s">
+      <c r="S17" s="74"/>
+      <c r="T17" s="74"/>
+      <c r="U17" s="74"/>
+      <c r="V17" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="W17" s="57"/>
-      <c r="X17" s="58" t="s">
+      <c r="W17" s="72"/>
+      <c r="X17" s="75" t="s">
         <v>59</v>
       </c>
-      <c r="Y17" s="58"/>
+      <c r="Y17" s="75"/>
     </row>
     <row r="18" spans="1:34" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
@@ -1527,8 +1524,8 @@
       <c r="Y19" s="6">
         <v>52954810.333279997</v>
       </c>
-      <c r="Z19" s="76">
-        <v>0.7</v>
+      <c r="Z19" s="6">
+        <v>70</v>
       </c>
       <c r="AA19" s="6"/>
       <c r="AB19" s="6"/>
@@ -1615,8 +1612,8 @@
       <c r="Y20" s="6">
         <v>0</v>
       </c>
-      <c r="Z20" s="76">
-        <v>0.8</v>
+      <c r="Z20" s="6">
+        <v>80</v>
       </c>
       <c r="AA20" s="6"/>
       <c r="AB20" s="6"/>
@@ -8763,7 +8760,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="I1:J8"/>
+    <mergeCell ref="R16:Y16"/>
+    <mergeCell ref="R17:U17"/>
+    <mergeCell ref="V17:W17"/>
+    <mergeCell ref="X17:Y17"/>
+    <mergeCell ref="L17:N17"/>
+    <mergeCell ref="O17:Q17"/>
+    <mergeCell ref="L16:Q16"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
@@ -8772,13 +8775,7 @@
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="A8:H8"/>
-    <mergeCell ref="R16:Y16"/>
-    <mergeCell ref="R17:U17"/>
-    <mergeCell ref="V17:W17"/>
-    <mergeCell ref="X17:Y17"/>
-    <mergeCell ref="L17:N17"/>
-    <mergeCell ref="O17:Q17"/>
-    <mergeCell ref="L16:Q16"/>
+    <mergeCell ref="I1:J8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
_ fix template kpi
</commit_message>
<xml_diff>
--- a/src/assets/resource/5002_KPIs Performance Report_202004_PBO_089_Final.xlsx
+++ b/src/assets/resource/5002_KPIs Performance Report_202004_PBO_089_Final.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hungm\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\salesapp-portal\src\assets\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -437,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -599,6 +599,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -650,17 +662,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -880,7 +883,7 @@
   <dimension ref="A1:AH221"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H11" workbookViewId="0">
-      <selection activeCell="Z16" sqref="Z16"/>
+      <selection activeCell="Z18" sqref="Z18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -906,19 +909,19 @@
   <sheetData>
     <row r="1" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="48"/>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="44"/>
       <c r="F1" s="44"/>
       <c r="G1" s="44"/>
       <c r="H1" s="45"/>
-      <c r="I1" s="66" t="s">
+      <c r="I1" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="67"/>
+      <c r="J1" s="71"/>
       <c r="K1" s="4"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -946,17 +949,17 @@
     </row>
     <row r="2" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="43"/>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
       <c r="H2" s="52"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="69"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="73"/>
       <c r="K2" s="4"/>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
@@ -984,17 +987,17 @@
     </row>
     <row r="3" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="49"/>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="16"/>
       <c r="H3" s="53"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="69"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="73"/>
       <c r="K3" s="4"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
@@ -1022,17 +1025,17 @@
     </row>
     <row r="4" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="50"/>
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="16"/>
       <c r="H4" s="53"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="69"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="73"/>
       <c r="K4" s="4"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
@@ -1067,8 +1070,8 @@
       <c r="F5" s="13"/>
       <c r="G5" s="16"/>
       <c r="H5" s="53"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="69"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="73"/>
       <c r="K5" s="4"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
@@ -1095,54 +1098,54 @@
       <c r="AH5" s="46"/>
     </row>
     <row r="6" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="69"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="73"/>
     </row>
     <row r="7" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="60" t="s">
+      <c r="A7" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="68"/>
-      <c r="J7" s="69"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="73"/>
     </row>
     <row r="8" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="63" t="s">
+      <c r="A8" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="64"/>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="65"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="71"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="69"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="75"/>
     </row>
     <row r="12" spans="1:34" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="59" t="s">
+      <c r="A12" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="59"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="63"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="7"/>
@@ -1304,24 +1307,24 @@
       <c r="I16" s="28"/>
       <c r="J16" s="29"/>
       <c r="K16" s="30"/>
-      <c r="L16" s="56" t="s">
+      <c r="L16" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="M16" s="56"/>
-      <c r="N16" s="56"/>
-      <c r="O16" s="56"/>
-      <c r="P16" s="56"/>
-      <c r="Q16" s="56"/>
-      <c r="R16" s="73" t="s">
+      <c r="M16" s="60"/>
+      <c r="N16" s="60"/>
+      <c r="O16" s="60"/>
+      <c r="P16" s="60"/>
+      <c r="Q16" s="60"/>
+      <c r="R16" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="S16" s="74"/>
-      <c r="T16" s="74"/>
-      <c r="U16" s="74"/>
-      <c r="V16" s="74"/>
-      <c r="W16" s="74"/>
-      <c r="X16" s="74"/>
-      <c r="Y16" s="74"/>
+      <c r="S16" s="56"/>
+      <c r="T16" s="56"/>
+      <c r="U16" s="56"/>
+      <c r="V16" s="56"/>
+      <c r="W16" s="56"/>
+      <c r="X16" s="56"/>
+      <c r="Y16" s="56"/>
     </row>
     <row r="17" spans="1:34" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
@@ -1335,30 +1338,30 @@
       <c r="I17" s="28"/>
       <c r="J17" s="29"/>
       <c r="K17" s="30"/>
-      <c r="L17" s="55" t="s">
+      <c r="L17" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="M17" s="55"/>
-      <c r="N17" s="55"/>
-      <c r="O17" s="55" t="s">
+      <c r="M17" s="59"/>
+      <c r="N17" s="59"/>
+      <c r="O17" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="P17" s="55"/>
-      <c r="Q17" s="55"/>
-      <c r="R17" s="73" t="s">
+      <c r="P17" s="59"/>
+      <c r="Q17" s="59"/>
+      <c r="R17" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="S17" s="74"/>
-      <c r="T17" s="74"/>
-      <c r="U17" s="74"/>
-      <c r="V17" s="72" t="s">
+      <c r="S17" s="56"/>
+      <c r="T17" s="56"/>
+      <c r="U17" s="56"/>
+      <c r="V17" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="W17" s="72"/>
-      <c r="X17" s="75" t="s">
+      <c r="W17" s="57"/>
+      <c r="X17" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="Y17" s="75"/>
+      <c r="Y17" s="58"/>
     </row>
     <row r="18" spans="1:34" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
@@ -1524,8 +1527,8 @@
       <c r="Y19" s="6">
         <v>52954810.333279997</v>
       </c>
-      <c r="Z19" s="6">
-        <v>70</v>
+      <c r="Z19" s="76">
+        <v>0.7</v>
       </c>
       <c r="AA19" s="6"/>
       <c r="AB19" s="6"/>
@@ -1612,8 +1615,8 @@
       <c r="Y20" s="6">
         <v>0</v>
       </c>
-      <c r="Z20" s="6">
-        <v>80</v>
+      <c r="Z20" s="76">
+        <v>0.8</v>
       </c>
       <c r="AA20" s="6"/>
       <c r="AB20" s="6"/>
@@ -8760,13 +8763,7 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="R16:Y16"/>
-    <mergeCell ref="R17:U17"/>
-    <mergeCell ref="V17:W17"/>
-    <mergeCell ref="X17:Y17"/>
-    <mergeCell ref="L17:N17"/>
-    <mergeCell ref="O17:Q17"/>
-    <mergeCell ref="L16:Q16"/>
+    <mergeCell ref="I1:J8"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
@@ -8775,7 +8772,13 @@
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="A8:H8"/>
-    <mergeCell ref="I1:J8"/>
+    <mergeCell ref="R16:Y16"/>
+    <mergeCell ref="R17:U17"/>
+    <mergeCell ref="V17:W17"/>
+    <mergeCell ref="X17:Y17"/>
+    <mergeCell ref="L17:N17"/>
+    <mergeCell ref="O17:Q17"/>
+    <mergeCell ref="L16:Q16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>